<commit_message>
Correcció de rutes related sic i sgde. Correcció del peu del comunicat
</commit_message>
<xml_diff>
--- a/static/related/sic/SIC-Formulari-Gestio-usuaris.xlsx
+++ b/static/related/sic/SIC-Formulari-Gestio-usuaris.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <workbookProtection workbookPassword="9D41" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="240" windowWidth="21312" windowHeight="9912"/>
+    <workbookView xWindow="120" yWindow="240" windowWidth="21315" windowHeight="9915"/>
   </bookViews>
   <sheets>
     <sheet name="Gestió d'usuaris" sheetId="2" r:id="rId1"/>
@@ -690,11 +690,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -704,35 +704,35 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -768,15 +768,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>2529840</xdr:colOff>
+          <xdr:colOff>2867025</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -809,15 +809,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1043940</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>220980</xdr:rowOff>
+          <xdr:colOff>1114425</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1139,28 +1139,28 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="B12" sqref="B12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="3" width="68.44140625" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="51"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D1" s="47"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>79</v>
       </c>
@@ -1168,15 +1168,15 @@
       <c r="C2" s="18"/>
       <c r="D2" s="19"/>
     </row>
-    <row r="3" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="47" t="s">
+    <row r="3" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="31"/>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>85</v>
       </c>
@@ -1192,7 +1192,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>77</v>
       </c>
@@ -1200,12 +1200,12 @@
       <c r="C6" s="26"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="47" t="s">
+    <row r="7" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
@@ -1223,7 +1223,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
@@ -1237,19 +1237,19 @@
       <c r="A11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>81</v>
       </c>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="D13" s="33"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>88</v>
       </c>
@@ -1269,29 +1269,29 @@
       </c>
       <c r="D14" s="33"/>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="39"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
@@ -1301,8 +1301,8 @@
       <c r="C18" s="40"/>
       <c r="D18" s="41"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="25" t="s">
@@ -1311,55 +1311,55 @@
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="44" t="s">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="48"/>
+      <c r="B20" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="48"/>
       <c r="B21" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
-      <c r="B22" s="45" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="48"/>
+      <c r="B22" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
-      <c r="B23" s="44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="48"/>
+      <c r="B23" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="44"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="43"/>
-      <c r="B24" s="46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="46"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -1367,7 +1367,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>72</v>
       </c>
@@ -1377,23 +1377,23 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="39"/>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="39"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="51"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>81</v>
       </c>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="D29" s="30"/>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>88</v>
       </c>
@@ -1413,29 +1413,29 @@
       </c>
       <c r="D30" s="30"/>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="39"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="51"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="39"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="51"/>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
@@ -1445,8 +1445,8 @@
       <c r="C34" s="40"/>
       <c r="D34" s="41"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="42" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
         <v>92</v>
       </c>
       <c r="B35" s="25" t="s">
@@ -1455,55 +1455,55 @@
       <c r="C35" s="22"/>
       <c r="D35" s="23"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="42"/>
-      <c r="B36" s="44" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="48"/>
+      <c r="B36" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="44"/>
+      <c r="C36" s="43"/>
       <c r="D36" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="42"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="48"/>
       <c r="B37" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="22"/>
       <c r="D37" s="23"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="42"/>
-      <c r="B38" s="45" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="48"/>
+      <c r="B38" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="44"/>
+      <c r="C38" s="43"/>
       <c r="D38" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="42"/>
-      <c r="B39" s="44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="48"/>
+      <c r="B39" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="44"/>
+      <c r="C39" s="43"/>
       <c r="D39" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="43"/>
-      <c r="B40" s="46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="49"/>
+      <c r="B40" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="46"/>
+      <c r="C40" s="44"/>
       <c r="D40" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
@@ -1511,7 +1511,7 @@
       <c r="C41" s="37"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>72</v>
       </c>
@@ -1521,23 +1521,23 @@
       </c>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="39"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="51"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="39"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="51"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>81</v>
       </c>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D45" s="33"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>88</v>
       </c>
@@ -1557,31 +1557,31 @@
       </c>
       <c r="D46" s="33"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="39"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="51"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="39"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="51"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="39"/>
-    </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="51"/>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
         <v>75</v>
       </c>
@@ -1589,8 +1589,8 @@
       <c r="C50" s="40"/>
       <c r="D50" s="41"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="42" t="s">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="48" t="s">
         <v>92</v>
       </c>
       <c r="B51" s="25" t="s">
@@ -1599,61 +1599,61 @@
       <c r="C51" s="22"/>
       <c r="D51" s="23"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="42"/>
-      <c r="B52" s="44" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="48"/>
+      <c r="B52" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="44"/>
+      <c r="C52" s="43"/>
       <c r="D52" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="42"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="48"/>
       <c r="B53" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C53" s="22"/>
       <c r="D53" s="23"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="42"/>
-      <c r="B54" s="45" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="48"/>
+      <c r="B54" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="44"/>
+      <c r="C54" s="43"/>
       <c r="D54" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="42"/>
-      <c r="B55" s="44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="48"/>
+      <c r="B55" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="44"/>
+      <c r="C55" s="43"/>
       <c r="D55" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="43"/>
-      <c r="B56" s="46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="49"/>
+      <c r="B56" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="46"/>
+      <c r="C56" s="44"/>
       <c r="D56" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
         <v>83</v>
       </c>
@@ -1661,22 +1661,14 @@
   </sheetData>
   <sheetProtection password="9D41" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="37">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="A51:A56"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="A19:A24"/>
@@ -1690,14 +1682,22 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="A51:A56"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22:D24 D20 D38:D40 D36 D54:D57 D52">
@@ -1711,44 +1711,44 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2057" r:id="rId4" name="combo_lots">
-          <controlPr defaultSize="0" autoLine="0" listFillRange="LOTS" r:id="rId5">
+        <control shapeId="2056" r:id="rId4" name="combo_ambits">
+          <controlPr defaultSize="0" autoLine="0" listFillRange="'Dades Formulari'!$B$2:$B$32" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>7620</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>7620</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1043940</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>2867025</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>220980</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2057" r:id="rId4" name="combo_lots"/>
+        <control shapeId="2056" r:id="rId4" name="combo_ambits"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2056" r:id="rId6" name="combo_ambits">
-          <controlPr defaultSize="0" autoLine="0" listFillRange="'Dades Formulari'!$B$2:$B$32" r:id="rId7">
+        <control shapeId="2057" r:id="rId6" name="combo_lots">
+          <controlPr defaultSize="0" autoLine="0" listFillRange="LOTS" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>7620</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>2529840</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1114425</xdr:colOff>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
@@ -1756,7 +1756,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2056" r:id="rId6" name="combo_ambits"/>
+        <control shapeId="2057" r:id="rId6" name="combo_lots"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -1772,24 +1772,24 @@
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" customWidth="1"/>
-    <col min="4" max="4" width="57.109375" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="51"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D1" s="47"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1797,7 +1797,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="52" t="s">
         <v>9</v>
@@ -1805,7 +1805,7 @@
       <c r="C3" s="53"/>
       <c r="D3" s="54"/>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1813,7 +1813,7 @@
       <c r="C4" s="15"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1829,7 +1829,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1845,7 +1845,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="7" t="s">
         <v>2</v>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
         <v>4</v>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="9" t="s">
         <v>6</v>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="D15" s="13"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>11</v>
       </c>
@@ -1938,12 +1938,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2064,92 +2064,92 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>63</v>
       </c>

</xml_diff>